<commit_message>
Se ejecuto el programa para verificar el funcionamiento tardio y movidas de dependencias
</commit_message>
<xml_diff>
--- a/paises_filtrados.xlsx
+++ b/paises_filtrados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,233 +478,233 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Antarctica</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>37950802</v>
       </c>
       <c r="C2" t="n">
-        <v>14000000</v>
+        <v>312679</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>121.37</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Antarctic</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Central Europe</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Polish</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>PLN (Polish złoty)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25687041</v>
+        <v>5530719</v>
       </c>
       <c r="C3" t="n">
-        <v>7692024</v>
+        <v>338424</v>
       </c>
       <c r="D3" t="n">
-        <v>3.34</v>
+        <v>16.34</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Australia and New Zealand</t>
+          <t>Northern Europe</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Finnish, Swedish</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AUD (Australian dollar)</t>
+          <t>EUR (Euro)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>106766</v>
+        <v>366425</v>
       </c>
       <c r="C4" t="n">
-        <v>180</v>
+        <v>103000</v>
       </c>
       <c r="D4" t="n">
-        <v>593.14</v>
+        <v>3.56</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Americas</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Caribbean</t>
+          <t>Northern Europe</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Dutch, Papiamento</t>
+          <t>Icelandic</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>AWG (Aruban florin)</t>
+          <t>ISK (Icelandic króna)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>40218234</v>
+        <v>8654622</v>
       </c>
       <c r="C5" t="n">
-        <v>652230</v>
+        <v>41284</v>
       </c>
       <c r="D5" t="n">
-        <v>61.66</v>
+        <v>209.64</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Southern Asia</t>
+          <t>Western Europe</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Dari, Pashto, Turkmen</t>
+          <t>French, Swiss German, Italian, Romansh</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>AFN (Afghan afghani)</t>
+          <t>CHF (Swiss franc)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Andorra</t>
+          <t>Christmas Island</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>77265</v>
+        <v>2072</v>
       </c>
       <c r="C6" t="n">
-        <v>468</v>
+        <v>135</v>
       </c>
       <c r="D6" t="n">
-        <v>165.1</v>
+        <v>15.35</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Southern Europe</t>
+          <t>Australia and New Zealand</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Catalan</t>
+          <t>English</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>EUR (Euro)</t>
+          <t>AUD (Australian dollar)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Antigua and Barbuda</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>97928</v>
+        <v>4994724</v>
       </c>
       <c r="C7" t="n">
-        <v>442</v>
+        <v>70273</v>
       </c>
       <c r="D7" t="n">
-        <v>221.56</v>
+        <v>71.08</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Americas</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Caribbean</t>
+          <t>Northern Europe</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>English, Irish</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>XCD (Eastern Caribbean dollar)</t>
+          <t>EUR (Euro)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Greenland</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45376763</v>
+        <v>56367</v>
       </c>
       <c r="C8" t="n">
-        <v>2780400</v>
+        <v>2166086</v>
       </c>
       <c r="D8" t="n">
-        <v>16.32</v>
+        <v>0.03</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -713,305 +713,161 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Guaraní, Spanish</t>
+          <t>Greenlandic</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ARS (Argentine peso)</t>
+          <t>DKK (krone)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>American Samoa</t>
+          <t>Bouvet Island</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>55197</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>199</v>
+        <v>49</v>
       </c>
       <c r="D9" t="n">
-        <v>277.37</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Antarctic</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Polynesia</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>English, Samoan</t>
+          <t>Norwegian</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>USD (United States dollar)</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Anguilla</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13452</v>
+        <v>5084300</v>
       </c>
       <c r="C10" t="n">
-        <v>91</v>
+        <v>270467</v>
       </c>
       <c r="D10" t="n">
-        <v>147.82</v>
+        <v>18.8</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Americas</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Caribbean</t>
+          <t>Australia and New Zealand</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>English, Māori, New Zealand Sign Language</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>XCD (Eastern Caribbean dollar)</t>
+          <t>NZD (New Zealand dollar)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Norfolk Island</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2963234</v>
+        <v>2302</v>
       </c>
       <c r="C11" t="n">
-        <v>29743</v>
+        <v>36</v>
       </c>
       <c r="D11" t="n">
-        <v>99.63</v>
+        <v>63.94</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Western Asia</t>
+          <t>Australia and New Zealand</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Armenian</t>
+          <t>English, Norfuk</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>AMD (Armenian dram)</t>
+          <t>AUD (Australian dollar)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Algeria</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44700000</v>
+        <v>69799978</v>
       </c>
       <c r="C12" t="n">
-        <v>2381741</v>
+        <v>513120</v>
       </c>
       <c r="D12" t="n">
-        <v>18.77</v>
+        <v>136.03</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Northern Africa</t>
+          <t>South-Eastern Asia</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Arabic</t>
+          <t>Thai</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>DZD (Algerian dinar)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Azerbaijan</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>10110116</v>
-      </c>
-      <c r="C13" t="n">
-        <v>86600</v>
-      </c>
-      <c r="D13" t="n">
-        <v>116.74</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Western Asia</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Azerbaijani</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>AZN (Azerbaijani manat)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Austria</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>8917205</v>
-      </c>
-      <c r="C14" t="n">
-        <v>83871</v>
-      </c>
-      <c r="D14" t="n">
-        <v>106.32</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Central Europe</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>German</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>EUR (Euro)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Albania</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2837743</v>
-      </c>
-      <c r="C15" t="n">
-        <v>28748</v>
-      </c>
-      <c r="D15" t="n">
-        <v>98.70999999999999</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Southeast Europe</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Albanian</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>ALL (Albanian lek)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Angola</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>32866268</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1246700</v>
-      </c>
-      <c r="D16" t="n">
-        <v>26.36</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Africa</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Middle Africa</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Portuguese</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>AOA (Angolan kwanza)</t>
+          <t>THB (Thai baht)</t>
         </is>
       </c>
     </row>

</xml_diff>